<commit_message>
added calculations of CPUE and allometric corrections
</commit_message>
<xml_diff>
--- a/Trawl CPUE no elasmobranch_mod.xlsx
+++ b/Trawl CPUE no elasmobranch_mod.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/MyPassport/SCMartin_eDNA/SCM_eDNA/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E86618F-0F6F-8444-AE6D-5BC03A70B952}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F4FF022-9F12-2244-ABB2-241159B0D6D6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="900" yWindow="460" windowWidth="32700" windowHeight="19640" xr2:uid="{D02D0B51-6D43-4C0F-9388-CD53AED06A2C}"/>
+    <workbookView xWindow="820" yWindow="460" windowWidth="27980" windowHeight="17540" activeTab="1" xr2:uid="{D02D0B51-6D43-4C0F-9388-CD53AED06A2C}"/>
   </bookViews>
   <sheets>
     <sheet name="CORRECT!" sheetId="2" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="39">
   <si>
     <t>American eel</t>
   </si>
@@ -505,7 +505,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6DD71312-C50A-4565-B5D3-5F3AD6629057}">
   <dimension ref="A1:AA56"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
@@ -5173,216 +5173,141 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{07981041-A9E4-9047-BCA6-810DA36D9AE3}">
-  <dimension ref="A1:D26"/>
+  <dimension ref="A1:A26"/>
   <sheetViews>
-    <sheetView zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:D26"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="2" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D5" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D6" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D7" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D8" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D9" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D10" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D11" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D12" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D13" s="2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="D14" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="D15" s="2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="D16" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="D17" s="2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D18" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="D19" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="D20" s="2" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="D21" s="2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="D22" s="2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="D23" s="2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A24" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="D24" s="2" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A25" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="D25" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A26" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="D26" s="2" t="s">
         <v>23</v>
       </c>
     </row>

</xml_diff>